<commit_message>
Added license & no-code alternative, fixed formats
</commit_message>
<xml_diff>
--- a/questions_with_gpt_answers.xlsx
+++ b/questions_with_gpt_answers.xlsx
@@ -563,11 +563,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
         </is>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2458,11 +2458,11 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>a</t>
         </is>
       </c>
       <c r="I45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -2998,11 +2998,11 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>c</t>
         </is>
       </c>
       <c r="I57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">

</xml_diff>